<commit_message>
Added surface pressure to list of things automatically grabbed from fort files
</commit_message>
<xml_diff>
--- a/Spectral-Processing/Spectra/eplanetpars.xlsx
+++ b/Spectral-Processing/Spectra/eplanetpars.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7BA129E-BDC3-418B-8618-6236C2EED71D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imalsky/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E074B3B-FA9A-0A41-9656-B9E73ADA918D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-43840" yWindow="-12240" windowWidth="39560" windowHeight="33300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -19,7 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="231">
   <si>
     <t>Name</t>
   </si>
@@ -712,13 +716,22 @@
   </si>
   <si>
     <t>Mass is upper limit, no quoted metallicity</t>
+  </si>
+  <si>
+    <t>55cnce</t>
+  </si>
+  <si>
+    <t>K0IV-V</t>
+  </si>
+  <si>
+    <t>Bourrier et al. 2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -785,6 +798,38 @@
       <sz val="11"/>
       <color rgb="FF1D1C1D"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF343A40"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF242424"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF333333"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="10">
@@ -876,10 +921,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -903,13 +949,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -925,8 +977,135 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>241300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="0.1737">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F1E8B44-9E44-3BB2-1E36-CC31B882CE3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4775200" y="11239500"/>
+          <a:ext cx="558800" cy="241300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>241300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="0.1737">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55C35A99-53F6-673C-00BC-7E0D55360690}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4775200" y="11239500"/>
+          <a:ext cx="558800" cy="241300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1214,7 +1393,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1224,29 +1403,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC09F8B8-526D-49BC-8E47-E6598E5B6377}">
   <dimension ref="A1:AS65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="F2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA2" sqref="AA2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R38" sqref="R38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="4" width="17.83203125" customWidth="1"/>
+    <col min="5" max="5" width="27.5" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.33203125" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="24" max="24" width="12.7109375" customWidth="1"/>
-    <col min="27" max="27" width="10.28515625" customWidth="1"/>
-    <col min="31" max="31" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="29.85546875" customWidth="1"/>
+    <col min="24" max="24" width="12.6640625" customWidth="1"/>
+    <col min="27" max="27" width="10.33203125" customWidth="1"/>
+    <col min="31" max="31" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1356,7 +1536,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1378,14 +1558,14 @@
       <c r="O2">
         <v>14.85</v>
       </c>
-      <c r="Y2" s="22">
+      <c r="Y2" s="21">
         <v>3250</v>
       </c>
-      <c r="AA2" s="23">
+      <c r="AA2" s="22">
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:45" ht="15.75">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -1411,7 +1591,7 @@
         <v>43</v>
       </c>
       <c r="I3">
-        <f>$G3/(E3)^2*AR$6</f>
+        <f t="shared" ref="I3:I34" si="0">$G3/(E3)^2*AR$6</f>
         <v>23.080962555134679</v>
       </c>
       <c r="J3">
@@ -1421,7 +1601,7 @@
         <v>43</v>
       </c>
       <c r="L3">
-        <f>$AR$9/(AR$10*J3)</f>
+        <f t="shared" ref="L3:L34" si="1">$AR$9/(AR$10*J3)</f>
         <v>3.2778692002319688E-5</v>
       </c>
       <c r="M3">
@@ -1453,7 +1633,7 @@
         <v>43</v>
       </c>
       <c r="W3">
-        <f>$Y3*(O3)^(-1/2)</f>
+        <f t="shared" ref="W3:W34" si="2">$Y3*(O3)^(-1/2)</f>
         <v>1709.166044641592</v>
       </c>
       <c r="Y3">
@@ -1487,7 +1667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:45" ht="15.75">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1513,7 +1693,7 @@
         <v>46</v>
       </c>
       <c r="I4">
-        <f>$G4/(E4)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>9.3650219295067547</v>
       </c>
       <c r="J4">
@@ -1523,7 +1703,7 @@
         <v>46</v>
       </c>
       <c r="L4">
-        <f>$AR$9/(AR$10*J4)</f>
+        <f t="shared" si="1"/>
         <v>2.0631840912781356E-5</v>
       </c>
       <c r="M4">
@@ -1555,7 +1735,7 @@
         <v>47</v>
       </c>
       <c r="W4">
-        <f>$Y4*(O4)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>2052.1100405717061</v>
       </c>
       <c r="Y4">
@@ -1594,12 +1774,12 @@
       <c r="AK4" t="s">
         <v>49</v>
       </c>
-      <c r="AR4" s="21" t="s">
+      <c r="AR4" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="AS4" s="21"/>
+      <c r="AS4" s="23"/>
     </row>
-    <row r="5" spans="1:45" ht="15.75">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -1623,7 +1803,7 @@
         <v>53</v>
       </c>
       <c r="I5">
-        <f>$G5/(E5)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>8.4302918807725202</v>
       </c>
       <c r="J5">
@@ -1633,7 +1813,7 @@
         <v>53</v>
       </c>
       <c r="L5">
-        <f>$AR$9/(AR$10*J5)</f>
+        <f t="shared" si="1"/>
         <v>5.704023659926043E-5</v>
       </c>
       <c r="M5">
@@ -1667,7 +1847,7 @@
         <v>53</v>
       </c>
       <c r="W5">
-        <f>$Y5*(O5)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>3333.6357925288753</v>
       </c>
       <c r="Y5">
@@ -1707,7 +1887,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:45" ht="15.75">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1733,7 +1913,7 @@
         <v>57</v>
       </c>
       <c r="I6">
-        <f>$G6/(E6)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>164.42669992195627</v>
       </c>
       <c r="J6">
@@ -1743,7 +1923,7 @@
         <v>57</v>
       </c>
       <c r="L6">
-        <f>$AR$9/(AR$10*J6)</f>
+        <f t="shared" si="1"/>
         <v>7.7244548208707726E-5</v>
       </c>
       <c r="M6">
@@ -1775,7 +1955,7 @@
         <v>57</v>
       </c>
       <c r="W6">
-        <f>$Y6*(O6)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>3447.9139120383484</v>
       </c>
       <c r="Y6">
@@ -1815,7 +1995,7 @@
         <v>24.786518999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -1841,7 +2021,7 @@
         <v>61</v>
       </c>
       <c r="I7">
-        <f>$G7/(E7)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>4.2577560037925446</v>
       </c>
       <c r="J7">
@@ -1851,7 +2031,7 @@
         <v>61</v>
       </c>
       <c r="L7">
-        <f>$AR$9/(AR$10*J7)</f>
+        <f t="shared" si="1"/>
         <v>1.7932621006804513E-5</v>
       </c>
       <c r="M7">
@@ -1883,7 +2063,7 @@
         <v>62</v>
       </c>
       <c r="W7">
-        <f>$Y7*(O7)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>1649.5832959136289</v>
       </c>
       <c r="Y7">
@@ -1920,7 +2100,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:45" ht="15.75">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -1946,7 +2126,7 @@
         <v>66</v>
       </c>
       <c r="I8">
-        <f>$G8/(E8)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>48.934489447015721</v>
       </c>
       <c r="J8">
@@ -1956,7 +2136,7 @@
         <v>66</v>
       </c>
       <c r="L8">
-        <f>$AR$9/(AR$10*J8)</f>
+        <f t="shared" si="1"/>
         <v>8.9396900371938392E-5</v>
       </c>
       <c r="M8">
@@ -1990,7 +2170,7 @@
         <v>66</v>
       </c>
       <c r="W8">
-        <f>$Y8*(O8)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>2018.5258680731547</v>
       </c>
       <c r="Y8">
@@ -2027,7 +2207,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:45" ht="15.75">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -2053,7 +2233,7 @@
         <v>71</v>
       </c>
       <c r="I9">
-        <f>$G9/(E9)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>6.8092799068350791</v>
       </c>
       <c r="J9">
@@ -2063,7 +2243,7 @@
         <v>71</v>
       </c>
       <c r="L9">
-        <f>$AR$9/(AR$10*J9)</f>
+        <f t="shared" si="1"/>
         <v>4.0180460076728808E-5</v>
       </c>
       <c r="M9">
@@ -2095,7 +2275,7 @@
         <v>71</v>
       </c>
       <c r="W9">
-        <f>$Y9*(O9)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>3085.9902658119458</v>
       </c>
       <c r="Y9">
@@ -2136,7 +2316,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:45">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -2159,7 +2339,7 @@
         <v>57</v>
       </c>
       <c r="I10">
-        <f>$G10/(E10)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>27.311208389847316</v>
       </c>
       <c r="J10">
@@ -2169,7 +2349,7 @@
         <v>57</v>
       </c>
       <c r="L10">
-        <f>$AR$9/(AR$10*J10)</f>
+        <f t="shared" si="1"/>
         <v>5.3470975077060064E-5</v>
       </c>
       <c r="M10">
@@ -2203,7 +2383,7 @@
         <v>57</v>
       </c>
       <c r="W10">
-        <f>$Y10*(O10)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>2432.5364325892365</v>
       </c>
       <c r="Y10">
@@ -2244,7 +2424,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:45" ht="15.75">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -2270,7 +2450,7 @@
         <v>76</v>
       </c>
       <c r="I11">
-        <f>$G11/(E11)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>13.361857575293012</v>
       </c>
       <c r="J11">
@@ -2280,7 +2460,7 @@
         <v>76</v>
       </c>
       <c r="L11">
-        <f>$AR$9/(AR$10*J11)</f>
+        <f t="shared" si="1"/>
         <v>2.3704547711846653E-5</v>
       </c>
       <c r="M11">
@@ -2314,7 +2494,7 @@
         <v>76</v>
       </c>
       <c r="W11">
-        <f>$Y11*(O11)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>1165.7710282303649</v>
       </c>
       <c r="Y11">
@@ -2348,7 +2528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:45" ht="15.75">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -2374,7 +2554,7 @@
         <v>80</v>
       </c>
       <c r="I12">
-        <f>$G12/(E12)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>4.5811093147466524</v>
       </c>
       <c r="J12">
@@ -2384,7 +2564,7 @@
         <v>80</v>
       </c>
       <c r="L12">
-        <f>$AR$9/(AR$10*J12)</f>
+        <f t="shared" si="1"/>
         <v>1.7173639718548801E-5</v>
       </c>
       <c r="M12">
@@ -2416,7 +2596,7 @@
         <v>80</v>
       </c>
       <c r="W12">
-        <f>$Y12*(O12)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>1404.8243222293909</v>
       </c>
       <c r="Y12">
@@ -2453,7 +2633,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:45" ht="15.75">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -2479,7 +2659,7 @@
         <v>84</v>
       </c>
       <c r="I13">
-        <f>$G13/(E13)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>12.830971573753461</v>
       </c>
       <c r="J13">
@@ -2489,7 +2669,7 @@
         <v>84</v>
       </c>
       <c r="L13">
-        <f>$AR$9/(AR$10*J13)</f>
+        <f t="shared" si="1"/>
         <v>4.2526053587414887E-5</v>
       </c>
       <c r="M13">
@@ -2523,7 +2703,7 @@
         <v>84</v>
       </c>
       <c r="W13">
-        <f>$Y13*(O13)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>2693.5108802581376</v>
       </c>
       <c r="Y13">
@@ -2566,7 +2746,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -2592,7 +2772,7 @@
         <v>89</v>
       </c>
       <c r="I14">
-        <f>$G14/(E14)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>34.043590130979283</v>
       </c>
       <c r="J14">
@@ -2602,7 +2782,7 @@
         <v>89</v>
       </c>
       <c r="L14">
-        <f>$AR$9/(AR$10*J14)</f>
+        <f t="shared" si="1"/>
         <v>7.5048936951724923E-5</v>
       </c>
       <c r="M14">
@@ -2636,7 +2816,7 @@
         <v>89</v>
       </c>
       <c r="W14">
-        <f>$Y14*(O14)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>3469.8032170895626</v>
       </c>
       <c r="Y14">
@@ -2667,7 +2847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>90</v>
       </c>
@@ -2687,7 +2867,7 @@
         <v>91</v>
       </c>
       <c r="I15">
-        <f>$G15/(E15)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>27.65614223374433</v>
       </c>
       <c r="J15">
@@ -2697,7 +2877,7 @@
         <v>91</v>
       </c>
       <c r="L15">
-        <f>$AR$9/(AR$10*J15)</f>
+        <f t="shared" si="1"/>
         <v>2.0932579442015239E-5</v>
       </c>
       <c r="M15">
@@ -2731,7 +2911,7 @@
         <v>91</v>
       </c>
       <c r="W15">
-        <f>$Y15*(O15)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>3201.2127082145762</v>
       </c>
       <c r="Y15">
@@ -2765,7 +2945,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:45" ht="15.75">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -2788,7 +2968,7 @@
         <v>3</v>
       </c>
       <c r="I16">
-        <f>$G16/(E16)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>24.532355618342098</v>
       </c>
       <c r="J16">
@@ -2798,7 +2978,7 @@
         <v>91</v>
       </c>
       <c r="L16">
-        <f>$AR$9/(AR$10*J16)</f>
+        <f t="shared" si="1"/>
         <v>2.0932579442015239E-5</v>
       </c>
       <c r="M16">
@@ -2832,7 +3012,7 @@
         <v>91</v>
       </c>
       <c r="W16">
-        <f>$Y16*(O16)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>3201.2127082145762</v>
       </c>
       <c r="Y16">
@@ -2863,7 +3043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:37" ht="15.75">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -2886,7 +3066,7 @@
         <v>0.3</v>
       </c>
       <c r="I17">
-        <f>$G17/(E17)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>2.4532355618342097</v>
       </c>
       <c r="J17">
@@ -2896,7 +3076,7 @@
         <v>91</v>
       </c>
       <c r="L17">
-        <f>$AR$9/(AR$10*J17)</f>
+        <f t="shared" si="1"/>
         <v>2.0932579442015239E-5</v>
       </c>
       <c r="M17">
@@ -2930,7 +3110,7 @@
         <v>91</v>
       </c>
       <c r="W17">
-        <f>$Y17*(O17)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>3201.2127082145762</v>
       </c>
       <c r="Y17">
@@ -2961,7 +3141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:37" ht="15.75">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -2987,7 +3167,7 @@
         <v>99</v>
       </c>
       <c r="I18">
-        <f>$G18/(E18)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>13.500230978486346</v>
       </c>
       <c r="J18">
@@ -2997,7 +3177,7 @@
         <v>99</v>
       </c>
       <c r="L18">
-        <f>$AR$9/(AR$10*J18)</f>
+        <f t="shared" si="1"/>
         <v>2.6591604364377628E-5</v>
       </c>
       <c r="M18">
@@ -3031,7 +3211,7 @@
         <v>99</v>
       </c>
       <c r="W18">
-        <f>$Y18*(O18)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>2897.4745928814359</v>
       </c>
       <c r="Y18">
@@ -3062,7 +3242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:37" ht="15.75">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>100</v>
       </c>
@@ -3086,7 +3266,7 @@
         <v>101</v>
       </c>
       <c r="I19">
-        <f>$G19/(E19)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>40.760053466666669</v>
       </c>
       <c r="J19">
@@ -3096,7 +3276,7 @@
         <v>101</v>
       </c>
       <c r="L19">
-        <f>$AR$9/(AR$10*J19)</f>
+        <f t="shared" si="1"/>
         <v>3.3843414480044674E-5</v>
       </c>
       <c r="M19">
@@ -3128,7 +3308,7 @@
         <v>101</v>
       </c>
       <c r="W19">
-        <f>$Y19*(O19)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>3599.9863405684982</v>
       </c>
       <c r="Y19">
@@ -3159,7 +3339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>102</v>
       </c>
@@ -3185,7 +3365,7 @@
         <v>104</v>
       </c>
       <c r="I20">
-        <f>$G20/(E20)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>24.550331154143791</v>
       </c>
       <c r="J20">
@@ -3195,7 +3375,7 @@
         <v>104</v>
       </c>
       <c r="L20">
-        <f>$AR$9/(AR$10*J20)</f>
+        <f t="shared" si="1"/>
         <v>5.1211840028099796E-5</v>
       </c>
       <c r="M20">
@@ -3229,7 +3409,7 @@
         <v>104</v>
       </c>
       <c r="W20">
-        <f>$Y20*(O20)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>2005.6814213186092</v>
       </c>
       <c r="Y20">
@@ -3260,7 +3440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>105</v>
       </c>
@@ -3286,7 +3466,7 @@
         <v>107</v>
       </c>
       <c r="I21">
-        <f>$G21/(E21)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>47.101992115292937</v>
       </c>
       <c r="J21">
@@ -3296,7 +3476,7 @@
         <v>107</v>
       </c>
       <c r="L21">
-        <f>$AR$9/(AR$10*J21)</f>
+        <f t="shared" si="1"/>
         <v>5.4387153032866055E-5</v>
       </c>
       <c r="M21">
@@ -3328,7 +3508,7 @@
         <v>107</v>
       </c>
       <c r="W21">
-        <f>$Y21*(O21)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>1824.5708341582933</v>
       </c>
       <c r="Y21">
@@ -3362,7 +3542,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="15.75">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>109</v>
       </c>
@@ -3388,7 +3568,7 @@
         <v>111</v>
       </c>
       <c r="I22">
-        <f>$G22/(E22)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>27.587116887127785</v>
       </c>
       <c r="J22">
@@ -3398,7 +3578,7 @@
         <v>111</v>
       </c>
       <c r="L22">
-        <f>$AR$9/(AR$10*J22)</f>
+        <f t="shared" si="1"/>
         <v>5.5675069623591714E-5</v>
       </c>
       <c r="M22">
@@ -3432,7 +3612,7 @@
         <v>112</v>
       </c>
       <c r="W22">
-        <f>$Y22*(O22)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>2317.1895475895785</v>
       </c>
       <c r="Y22">
@@ -3466,7 +3646,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:37" ht="15.75">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>114</v>
       </c>
@@ -3492,7 +3672,7 @@
         <v>116</v>
       </c>
       <c r="I23">
-        <f>$G23/(E23)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>3.3662090086011767</v>
       </c>
       <c r="J23">
@@ -3502,7 +3682,7 @@
         <v>116</v>
       </c>
       <c r="L23">
-        <f>$AR$9/(AR$10*J23)</f>
+        <f t="shared" si="1"/>
         <v>1.2710334574810126E-5</v>
       </c>
       <c r="M23">
@@ -3536,7 +3716,7 @@
         <v>116</v>
       </c>
       <c r="W23">
-        <f>$Y23*(O23)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>1038.4080165287673</v>
       </c>
       <c r="Y23">
@@ -3570,7 +3750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="15.75">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -3596,7 +3776,7 @@
         <v>119</v>
       </c>
       <c r="I24">
-        <f>$G24/(E24)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>29.166235706018519</v>
       </c>
       <c r="J24">
@@ -3606,7 +3786,7 @@
         <v>119</v>
       </c>
       <c r="L24">
-        <f>$AR$9/(AR$10*J24)</f>
+        <f t="shared" si="1"/>
         <v>3.2523519143334644E-5</v>
       </c>
       <c r="M24">
@@ -3638,7 +3818,7 @@
         <v>119</v>
       </c>
       <c r="W24">
-        <f>$Y24*(O24)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>1861.6265416212921</v>
       </c>
       <c r="Y24">
@@ -3669,7 +3849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>120</v>
       </c>
@@ -3695,7 +3875,7 @@
         <v>122</v>
       </c>
       <c r="I25">
-        <f>$G25/(E25)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>9.4922842179521627</v>
       </c>
       <c r="J25">
@@ -3705,7 +3885,7 @@
         <v>122</v>
       </c>
       <c r="L25">
-        <f>$AR$9/(AR$10*J25)</f>
+        <f t="shared" si="1"/>
         <v>1.6842860629685281E-5</v>
       </c>
       <c r="M25">
@@ -3737,7 +3917,7 @@
         <v>122</v>
       </c>
       <c r="W25">
-        <f>$Y25*(O25)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>1637.5672315503318</v>
       </c>
       <c r="Y25">
@@ -3771,7 +3951,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="15.75">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>124</v>
       </c>
@@ -3797,7 +3977,7 @@
         <v>126</v>
       </c>
       <c r="I26">
-        <f>$G26/(E26)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>5.7681814349352747</v>
       </c>
       <c r="J26">
@@ -3807,7 +3987,7 @@
         <v>126</v>
       </c>
       <c r="L26">
-        <f>$AR$9/(AR$10*J26)</f>
+        <f t="shared" si="1"/>
         <v>1.8800272484170911E-5</v>
       </c>
       <c r="M26">
@@ -3839,7 +4019,7 @@
         <v>126</v>
       </c>
       <c r="W26">
-        <f>$Y26*(O26)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>1362.9067139401391</v>
       </c>
       <c r="Y26">
@@ -3873,7 +4053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="15.75">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>127</v>
       </c>
@@ -3899,7 +4079,7 @@
         <v>129</v>
       </c>
       <c r="I27">
-        <f>$G27/(E27)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>10.386312151484161</v>
       </c>
       <c r="J27">
@@ -3909,7 +4089,7 @@
         <v>129</v>
       </c>
       <c r="L27">
-        <f>$AR$9/(AR$10*J27)</f>
+        <f t="shared" si="1"/>
         <v>3.4018121513787258E-5</v>
       </c>
       <c r="M27">
@@ -3941,7 +4121,7 @@
         <v>130</v>
       </c>
       <c r="W27">
-        <f>$Y27*(O27)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>2725.6314654762814</v>
       </c>
       <c r="Y27">
@@ -3978,7 +4158,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="15.75">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>132</v>
       </c>
@@ -4004,7 +4184,7 @@
         <v>134</v>
       </c>
       <c r="I28">
-        <f>$G28/(E28)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>20.383149290349021</v>
       </c>
       <c r="J28">
@@ -4014,7 +4194,7 @@
         <v>134</v>
       </c>
       <c r="L28">
-        <f>$AR$9/(AR$10*J28)</f>
+        <f t="shared" si="1"/>
         <v>3.3287385419433661E-5</v>
       </c>
       <c r="M28">
@@ -4046,7 +4226,7 @@
         <v>134</v>
       </c>
       <c r="W28">
-        <f>$Y28*(O28)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>2208.1935573447736</v>
       </c>
       <c r="Y28">
@@ -4080,7 +4260,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="15.75">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>135</v>
       </c>
@@ -4106,7 +4286,7 @@
         <v>136</v>
       </c>
       <c r="I29">
-        <f>$G29/(E29)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>7.6229041089662619</v>
       </c>
       <c r="J29">
@@ -4116,7 +4296,7 @@
         <v>136</v>
       </c>
       <c r="L29">
-        <f>$AR$9/(AR$10*J29)</f>
+        <f t="shared" si="1"/>
         <v>4.1560616647066365E-5</v>
       </c>
       <c r="M29">
@@ -4148,7 +4328,7 @@
         <v>137</v>
       </c>
       <c r="W29">
-        <f>$Y29*(O29)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>1850.7097907800128</v>
       </c>
       <c r="Y29">
@@ -4185,7 +4365,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="1:37" ht="15.75">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>139</v>
       </c>
@@ -4211,7 +4391,7 @@
         <v>140</v>
       </c>
       <c r="I30">
-        <f>$G30/(E30)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>34.247040621395612</v>
       </c>
       <c r="J30">
@@ -4221,7 +4401,7 @@
         <v>140</v>
       </c>
       <c r="L30">
-        <f>$AR$9/(AR$10*J30)</f>
+        <f t="shared" si="1"/>
         <v>5.9958017352846601E-5</v>
       </c>
       <c r="M30">
@@ -4255,7 +4435,7 @@
         <v>141</v>
       </c>
       <c r="W30">
-        <f>$Y30*(O30)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>2760.1744294224741</v>
       </c>
       <c r="Y30">
@@ -4292,7 +4472,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:37" ht="15.75">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -4316,7 +4496,7 @@
         <v>144</v>
       </c>
       <c r="I31">
-        <f>$G31/(E31)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>21.923741242008557</v>
       </c>
       <c r="J31">
@@ -4326,7 +4506,7 @@
         <v>144</v>
       </c>
       <c r="L31">
-        <f>$AR$9/(AR$10*J31)</f>
+        <f t="shared" si="1"/>
         <v>3.2984480662137684E-5</v>
       </c>
       <c r="M31">
@@ -4358,7 +4538,7 @@
         <v>144</v>
       </c>
       <c r="W31">
-        <f>$Y31*(O31)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>3115.403788119293</v>
       </c>
       <c r="Y31">
@@ -4389,7 +4569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:37" ht="15.75">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -4415,7 +4595,7 @@
         <v>46</v>
       </c>
       <c r="I32">
-        <f>$G32/(E32)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>17.200287107377648</v>
       </c>
       <c r="J32">
@@ -4425,7 +4605,7 @@
         <v>46</v>
       </c>
       <c r="L32">
-        <f>$AR$9/(AR$10*J32)</f>
+        <f t="shared" si="1"/>
         <v>2.5287678226306649E-5</v>
       </c>
       <c r="M32">
@@ -4457,7 +4637,7 @@
         <v>147</v>
       </c>
       <c r="W32">
-        <f>$Y32*(O32)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>2369.5383330439508</v>
       </c>
       <c r="Y32">
@@ -4494,7 +4674,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="1:36">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>149</v>
       </c>
@@ -4520,7 +4700,7 @@
         <v>151</v>
       </c>
       <c r="I33">
-        <f>$G33/(E33)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>15.818128490686933</v>
       </c>
       <c r="J33">
@@ -4530,7 +4710,7 @@
         <v>151</v>
       </c>
       <c r="L33">
-        <f>$AR$9/(AR$10*J33)</f>
+        <f t="shared" si="1"/>
         <v>7.8572395597855519E-5</v>
       </c>
       <c r="M33">
@@ -4564,7 +4744,7 @@
         <v>151</v>
       </c>
       <c r="W33">
-        <f>$Y33*(O33)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>3540.6162929707161</v>
       </c>
       <c r="Y33">
@@ -4595,7 +4775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:36" ht="15.75">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>152</v>
       </c>
@@ -4621,7 +4801,7 @@
         <v>136</v>
       </c>
       <c r="I34" s="6">
-        <f>$G34/(E34)^2*AR$6</f>
+        <f t="shared" si="0"/>
         <v>10.562561572141355</v>
       </c>
       <c r="J34" s="6">
@@ -4631,7 +4811,7 @@
         <v>136</v>
       </c>
       <c r="L34" s="6">
-        <f>$AR$9/(AR$10*J34)</f>
+        <f t="shared" si="1"/>
         <v>6.6630681891021408E-5</v>
       </c>
       <c r="M34" s="6">
@@ -4664,7 +4844,7 @@
         <v>154</v>
       </c>
       <c r="W34" s="6">
-        <f>$Y34*(O34)^(-1/2)</f>
+        <f t="shared" si="2"/>
         <v>3678.6165294041898</v>
       </c>
       <c r="X34" s="6"/>
@@ -4700,7 +4880,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35" spans="1:36">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>156</v>
       </c>
@@ -4726,7 +4906,7 @@
         <v>158</v>
       </c>
       <c r="I35" s="8">
-        <f>$G35/(E35)^2*AR$6</f>
+        <f t="shared" ref="I35:I60" si="3">$G35/(E35)^2*AR$6</f>
         <v>122.35280905957336</v>
       </c>
       <c r="J35">
@@ -4736,7 +4916,7 @@
         <v>158</v>
       </c>
       <c r="L35">
-        <f>$AR$9/(AR$10*J35)</f>
+        <f t="shared" ref="L35:L59" si="4">$AR$9/(AR$10*J35)</f>
         <v>3.2410718573946517E-5</v>
       </c>
       <c r="M35">
@@ -4770,7 +4950,7 @@
         <v>158</v>
       </c>
       <c r="W35">
-        <f>$Y35*(O35)^(-1/2)</f>
+        <f t="shared" ref="W35:W59" si="5">$Y35*(O35)^(-1/2)</f>
         <v>2647.8244051046054</v>
       </c>
       <c r="Y35">
@@ -4801,7 +4981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:36" ht="15.75">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>159</v>
       </c>
@@ -4827,7 +5007,7 @@
         <v>57</v>
       </c>
       <c r="I36">
-        <f>$G36/(E36)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>14.285928367690941</v>
       </c>
       <c r="J36">
@@ -4837,7 +5017,7 @@
         <v>57</v>
       </c>
       <c r="L36">
-        <f>$AR$9/(AR$10*J36)</f>
+        <f t="shared" si="4"/>
         <v>9.2188769086010649E-5</v>
       </c>
       <c r="M36">
@@ -4869,7 +5049,7 @@
         <v>57</v>
       </c>
       <c r="W36">
-        <f>$Y36*(O36)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>2987.8258502853159</v>
       </c>
       <c r="Y36">
@@ -4900,7 +5080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:36" ht="15.75">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>161</v>
       </c>
@@ -4924,7 +5104,7 @@
         <v>154</v>
       </c>
       <c r="I37">
-        <f>$G37/(E37)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>20.443404216658806</v>
       </c>
       <c r="J37">
@@ -4934,7 +5114,7 @@
         <v>154</v>
       </c>
       <c r="L37">
-        <f>$AR$9/(AR$10*J37)</f>
+        <f t="shared" si="4"/>
         <v>5.9614591855222603E-5</v>
       </c>
       <c r="M37">
@@ -4968,7 +5148,7 @@
         <v>154</v>
       </c>
       <c r="W37">
-        <f>$Y37*(O37)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>3931.8223646615656</v>
       </c>
       <c r="Y37">
@@ -5002,7 +5182,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:36">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>163</v>
       </c>
@@ -5022,7 +5202,7 @@
         <v>165</v>
       </c>
       <c r="I38">
-        <f>$G38/(E38)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>19.962961496761217</v>
       </c>
       <c r="J38">
@@ -5032,7 +5212,7 @@
         <v>165</v>
       </c>
       <c r="L38">
-        <f>$AR$9/(AR$10*J38)</f>
+        <f t="shared" si="4"/>
         <v>4.9099249432225199E-5</v>
       </c>
       <c r="M38">
@@ -5066,7 +5246,7 @@
         <v>165</v>
       </c>
       <c r="W38">
-        <f>$Y38*(O38)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>5727.4191536634298</v>
       </c>
       <c r="Y38">
@@ -5097,7 +5277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:36">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>166</v>
       </c>
@@ -5120,7 +5300,7 @@
         <v>46</v>
       </c>
       <c r="I39" s="8">
-        <f>$G39/(E39)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>196.74299456249997</v>
       </c>
       <c r="J39">
@@ -5130,7 +5310,7 @@
         <v>46</v>
       </c>
       <c r="L39">
-        <f>$AR$9/(AR$10*J39)</f>
+        <f t="shared" si="4"/>
         <v>1.2908926854395317E-5</v>
       </c>
       <c r="M39">
@@ -5162,7 +5342,7 @@
         <v>168</v>
       </c>
       <c r="W39">
-        <f>$Y39*(O39)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>2056.6499589132668</v>
       </c>
       <c r="Y39">
@@ -5196,7 +5376,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="40" spans="1:36" ht="15.75">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>170</v>
       </c>
@@ -5222,7 +5402,7 @@
         <v>46</v>
       </c>
       <c r="I40" s="8">
-        <f>$G40/(E40)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>90.887643232231781</v>
       </c>
       <c r="J40">
@@ -5232,7 +5412,7 @@
         <v>46</v>
       </c>
       <c r="L40">
-        <f>$AR$9/(AR$10*J40)</f>
+        <f t="shared" si="4"/>
         <v>2.2785881476162105E-5</v>
       </c>
       <c r="M40">
@@ -5264,7 +5444,7 @@
         <v>112</v>
       </c>
       <c r="W40">
-        <f>$Y40*(O40)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>2889.6206105174556</v>
       </c>
       <c r="Y40">
@@ -5298,7 +5478,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:36">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>171</v>
       </c>
@@ -5318,7 +5498,7 @@
         <v>173</v>
       </c>
       <c r="I41">
-        <f>$G41/(E41)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>14.802782406163217</v>
       </c>
       <c r="J41">
@@ -5328,7 +5508,7 @@
         <v>173</v>
       </c>
       <c r="L41">
-        <f>$AR$9/(AR$10*J41)</f>
+        <f t="shared" si="4"/>
         <v>2.7505619105299004E-5</v>
       </c>
       <c r="M41">
@@ -5362,7 +5542,7 @@
         <v>173</v>
       </c>
       <c r="W41">
-        <f>$Y41*(O41)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>895.85074410215827</v>
       </c>
       <c r="Y41">
@@ -5393,7 +5573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:36">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>174</v>
       </c>
@@ -5413,7 +5593,7 @@
         <v>136</v>
       </c>
       <c r="I42">
-        <f>$G42/(E42)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>5.807183768394661</v>
       </c>
       <c r="J42">
@@ -5423,7 +5603,7 @@
         <v>136</v>
       </c>
       <c r="L42">
-        <f>$AR$9/(AR$10*J42)</f>
+        <f t="shared" si="4"/>
         <v>2.263328406451387E-5</v>
       </c>
       <c r="M42">
@@ -5455,7 +5635,7 @@
         <v>176</v>
       </c>
       <c r="W42">
-        <f>$Y42*(O42)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>1379.3908485227762</v>
       </c>
       <c r="Y42">
@@ -5489,7 +5669,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="43" spans="1:36">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>178</v>
       </c>
@@ -5509,7 +5689,7 @@
         <v>179</v>
       </c>
       <c r="I43">
-        <f>$G43/(E43)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>7.4797184642028425</v>
       </c>
       <c r="J43">
@@ -5519,7 +5699,7 @@
         <v>179</v>
       </c>
       <c r="L43">
-        <f>$AR$9/(AR$10*J43)</f>
+        <f t="shared" si="4"/>
         <v>1.6286040372445322E-5</v>
       </c>
       <c r="M43">
@@ -5553,7 +5733,7 @@
         <v>179</v>
       </c>
       <c r="W43">
-        <f>$Y43*(O43)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>1905.0963396455745</v>
       </c>
       <c r="Y43">
@@ -5584,7 +5764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:36">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>180</v>
       </c>
@@ -5604,7 +5784,7 @@
         <v>181</v>
       </c>
       <c r="I44">
-        <f>$G44/(E44)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>5.9560399340239067</v>
       </c>
       <c r="J44">
@@ -5614,7 +5794,7 @@
         <v>181</v>
       </c>
       <c r="L44">
-        <f>$AR$9/(AR$10*J44)</f>
+        <f t="shared" si="4"/>
         <v>9.9239320640361575E-6</v>
       </c>
       <c r="M44">
@@ -5648,7 +5828,7 @@
         <v>181</v>
       </c>
       <c r="W44">
-        <f>$Y44*(O44)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>1045.8037406234125</v>
       </c>
       <c r="Y44">
@@ -5679,7 +5859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:36">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>182</v>
       </c>
@@ -5695,7 +5875,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45">
-        <f>$G45/(E45)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J45">
@@ -5705,7 +5885,7 @@
         <v>183</v>
       </c>
       <c r="L45">
-        <f>$AR$9/(AR$10*J45)</f>
+        <f t="shared" si="4"/>
         <v>1.04493168788677E-5</v>
       </c>
       <c r="M45">
@@ -5737,7 +5917,7 @@
         <v>183</v>
       </c>
       <c r="W45">
-        <f>$Y45*(O45)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>1659.1014198557971</v>
       </c>
       <c r="Y45">
@@ -5771,7 +5951,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="46" spans="1:36">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>186</v>
       </c>
@@ -5791,7 +5971,7 @@
         <v>187</v>
       </c>
       <c r="I46">
-        <f>$G46/(E46)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>36.906013379934912</v>
       </c>
       <c r="J46">
@@ -5801,7 +5981,7 @@
         <v>187</v>
       </c>
       <c r="L46">
-        <f>$AR$9/(AR$10*J46)</f>
+        <f t="shared" si="4"/>
         <v>9.4826683004114247E-5</v>
       </c>
       <c r="M46">
@@ -5831,7 +6011,7 @@
         <v>187</v>
       </c>
       <c r="W46">
-        <f>$Y46*(O46)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>2181.3445390861652</v>
       </c>
       <c r="Y46">
@@ -5865,7 +6045,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="47" spans="1:36">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>189</v>
       </c>
@@ -5885,7 +6065,7 @@
         <v>190</v>
       </c>
       <c r="I47">
-        <f>$G47/(E47)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>2.3770970323405609</v>
       </c>
       <c r="J47">
@@ -5895,7 +6075,7 @@
         <v>190</v>
       </c>
       <c r="L47">
-        <f>$AR$9/(AR$10*J47)</f>
+        <f t="shared" si="4"/>
         <v>1.7405690046349336E-5</v>
       </c>
       <c r="M47">
@@ -5927,7 +6107,7 @@
         <v>190</v>
       </c>
       <c r="W47">
-        <f>$Y47*(O47)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>1981.4836663607048</v>
       </c>
       <c r="Y47">
@@ -5961,7 +6141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:36">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>191</v>
       </c>
@@ -5981,7 +6161,7 @@
         <v>192</v>
       </c>
       <c r="I48">
-        <f>$G48/(E48)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>6.3074790098261513</v>
       </c>
       <c r="J48">
@@ -5991,7 +6171,7 @@
         <v>192</v>
       </c>
       <c r="L48">
-        <f>$AR$9/(AR$10*J48)</f>
+        <f t="shared" si="4"/>
         <v>1.3359330907172611E-5</v>
       </c>
       <c r="M48">
@@ -6025,7 +6205,7 @@
         <v>192</v>
       </c>
       <c r="W48">
-        <f>$Y48*(O48)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>1799.7664548589069</v>
       </c>
       <c r="Y48">
@@ -6056,7 +6236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:36">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>193</v>
       </c>
@@ -6076,7 +6256,7 @@
         <v>192</v>
       </c>
       <c r="I49">
-        <f>$G49/(E49)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>9.9846202382974564E-2</v>
       </c>
       <c r="J49">
@@ -6086,7 +6266,7 @@
         <v>192</v>
       </c>
       <c r="L49">
-        <f>$AR$9/(AR$10*J49)</f>
+        <f t="shared" si="4"/>
         <v>2.1741638522402687E-5</v>
       </c>
       <c r="M49">
@@ -6120,7 +6300,7 @@
         <v>192</v>
       </c>
       <c r="W49">
-        <f>$Y49*(O49)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>3495.5560550349087</v>
       </c>
       <c r="Y49">
@@ -6154,7 +6334,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="50" spans="1:36">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>195</v>
       </c>
@@ -6174,7 +6354,7 @@
         <v>196</v>
       </c>
       <c r="I50">
-        <f>$G50/(E50)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>3.0388501733440858</v>
       </c>
       <c r="J50">
@@ -6184,7 +6364,7 @@
         <v>196</v>
       </c>
       <c r="L50">
-        <f>$AR$9/(AR$10*J50)</f>
+        <f t="shared" si="4"/>
         <v>1.9468145948729546E-5</v>
       </c>
       <c r="M50">
@@ -6216,7 +6396,7 @@
         <v>196</v>
       </c>
       <c r="W50">
-        <f>$Y50*(O50)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>2505.4904660367934</v>
       </c>
       <c r="Y50">
@@ -6250,7 +6430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:36">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>197</v>
       </c>
@@ -6270,7 +6450,7 @@
         <v>46</v>
       </c>
       <c r="I51">
-        <f>$G51/(E51)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>4.6129530858608723</v>
       </c>
       <c r="J51">
@@ -6280,7 +6460,7 @@
         <v>46</v>
       </c>
       <c r="L51">
-        <f>$AR$9/(AR$10*J51)</f>
+        <f t="shared" si="4"/>
         <v>1.661048956767131E-5</v>
       </c>
       <c r="M51">
@@ -6312,7 +6492,7 @@
         <v>112</v>
       </c>
       <c r="W51">
-        <f>$Y51*(O51)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>2161.9730492902449</v>
       </c>
       <c r="Y51">
@@ -6346,7 +6526,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="52" spans="1:36">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>199</v>
       </c>
@@ -6366,7 +6546,7 @@
         <v>46</v>
       </c>
       <c r="I52">
-        <f>$G52/(E52)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>94.824834675517494</v>
       </c>
       <c r="J52">
@@ -6376,7 +6556,7 @@
         <v>46</v>
       </c>
       <c r="L52">
-        <f>$AR$9/(AR$10*J52)</f>
+        <f t="shared" si="4"/>
         <v>6.5258619616724466E-7</v>
       </c>
       <c r="M52">
@@ -6408,7 +6588,7 @@
         <v>201</v>
       </c>
       <c r="W52">
-        <f>$Y52*(O52)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>560.65988804534697</v>
       </c>
       <c r="Y52">
@@ -6442,7 +6622,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:36">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>203</v>
       </c>
@@ -6462,7 +6642,7 @@
         <v>205</v>
       </c>
       <c r="I53">
-        <f>$G53/(E53)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>8.1948145780012691</v>
       </c>
       <c r="J53">
@@ -6472,7 +6652,7 @@
         <v>205</v>
       </c>
       <c r="L53">
-        <f>$AR$9/(AR$10*J53)</f>
+        <f t="shared" si="4"/>
         <v>2.1794936226864255E-5</v>
       </c>
       <c r="M53">
@@ -6504,7 +6684,7 @@
         <v>206</v>
       </c>
       <c r="W53">
-        <f>$Y53*(O53)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>1016.0135783203241</v>
       </c>
       <c r="Y53">
@@ -6538,7 +6718,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="54" spans="1:36">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>208</v>
       </c>
@@ -6558,7 +6738,7 @@
         <v>210</v>
       </c>
       <c r="I54">
-        <f>$G54/(E54)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>1.0165812650448467</v>
       </c>
       <c r="J54">
@@ -6568,7 +6748,7 @@
         <v>210</v>
       </c>
       <c r="L54">
-        <f>$AR$9/(AR$10*J54)</f>
+        <f t="shared" si="4"/>
         <v>8.9353400624707128E-6</v>
       </c>
       <c r="M54">
@@ -6600,7 +6780,7 @@
         <v>210</v>
       </c>
       <c r="W54">
-        <f>$Y54*(O54)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>1257.5982045463766</v>
       </c>
       <c r="Y54">
@@ -6634,7 +6814,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="55" spans="1:36">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>213</v>
       </c>
@@ -6654,7 +6834,7 @@
         <v>214</v>
       </c>
       <c r="I55">
-        <f>$G55/(E55)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>0.62285029831427863</v>
       </c>
       <c r="J55">
@@ -6664,7 +6844,7 @@
         <v>214</v>
       </c>
       <c r="L55">
-        <f>$AR$9/(AR$10*J55)</f>
+        <f t="shared" si="4"/>
         <v>5.5860760817478567E-7</v>
       </c>
       <c r="M55">
@@ -6696,7 +6876,7 @@
         <v>214</v>
       </c>
       <c r="W55">
-        <f>$Y55*(O55)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>507.34319517872251</v>
       </c>
       <c r="Y55">
@@ -6727,7 +6907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:36">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>215</v>
       </c>
@@ -6747,7 +6927,7 @@
         <v>216</v>
       </c>
       <c r="I56">
-        <f>$G56/(E56)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>12.900832074689264</v>
       </c>
       <c r="J56">
@@ -6757,7 +6937,7 @@
         <v>216</v>
       </c>
       <c r="L56">
-        <f>$AR$9/(AR$10*J56)</f>
+        <f t="shared" si="4"/>
         <v>9.1814744696598711E-5</v>
       </c>
       <c r="M56">
@@ -6790,7 +6970,7 @@
       </c>
       <c r="V56" s="2"/>
       <c r="W56">
-        <f>$Y56*(O56)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>2764.3334806908529</v>
       </c>
       <c r="Y56">
@@ -6824,7 +7004,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="57" spans="1:36">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>218</v>
       </c>
@@ -6844,7 +7024,7 @@
         <v>219</v>
       </c>
       <c r="I57">
-        <f>$G57/(E57)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>11.150796300140872</v>
       </c>
       <c r="J57">
@@ -6854,7 +7034,7 @@
         <v>219</v>
       </c>
       <c r="L57">
-        <f>$AR$9/(AR$10*J57)</f>
+        <f t="shared" si="4"/>
         <v>3.0125624354351517E-6</v>
       </c>
       <c r="M57">
@@ -6888,7 +7068,7 @@
         <v>219</v>
       </c>
       <c r="W57">
-        <f>$Y57*(O57)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>956.4769459574801</v>
       </c>
       <c r="Y57">
@@ -6922,7 +7102,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="58" spans="1:36">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>222</v>
       </c>
@@ -6936,7 +7116,7 @@
         <v>219</v>
       </c>
       <c r="I58">
-        <f>$G58/(E58)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J58">
@@ -6946,7 +7126,7 @@
         <v>219</v>
       </c>
       <c r="L58">
-        <f>$AR$9/(AR$10*J58)</f>
+        <f t="shared" si="4"/>
         <v>8.815242977997717E-6</v>
       </c>
       <c r="M58">
@@ -6980,7 +7160,7 @@
         <v>219</v>
       </c>
       <c r="W58">
-        <f>$Y58*(O58)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>1368.4659346892242</v>
       </c>
       <c r="Y58">
@@ -7014,7 +7194,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="59" spans="1:36">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>225</v>
       </c>
@@ -7034,7 +7214,7 @@
         <v>226</v>
       </c>
       <c r="I59">
-        <f>$G59/(E59)^2*AR$6</f>
+        <f t="shared" si="3"/>
         <v>397.19033586318363</v>
       </c>
       <c r="J59">
@@ -7044,7 +7224,7 @@
         <v>226</v>
       </c>
       <c r="L59">
-        <f>$AR$9/(AR$10*J59)</f>
+        <f t="shared" si="4"/>
         <v>5.165136748778119E-5</v>
       </c>
       <c r="M59">
@@ -7078,7 +7258,7 @@
         <v>226</v>
       </c>
       <c r="W59">
-        <f>$Y59*(O59)^(-1/2)</f>
+        <f t="shared" si="5"/>
         <v>256.95156575288104</v>
       </c>
       <c r="Y59">
@@ -7106,7 +7286,70 @@
         <v>227</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="60" spans="1:36" ht="21" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>228</v>
+      </c>
+      <c r="B60" t="s">
+        <v>37</v>
+      </c>
+      <c r="D60" t="s">
+        <v>229</v>
+      </c>
+      <c r="E60">
+        <v>0.17369999999999999</v>
+      </c>
+      <c r="F60" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="G60">
+        <v>2.7036000000000001E-2</v>
+      </c>
+      <c r="H60" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="I60">
+        <f>$G60/(E60)^2*AR$6</f>
+        <v>22.210500229983804</v>
+      </c>
+      <c r="J60" s="26">
+        <v>0.73654739999999996</v>
+      </c>
+      <c r="L60">
+        <v>9.8739436577609206E-5</v>
+      </c>
+      <c r="M60" s="27">
+        <v>1.54E-2</v>
+      </c>
+      <c r="O60" s="24">
+        <v>3.52</v>
+      </c>
+      <c r="Q60">
+        <v>0.05</v>
+      </c>
+      <c r="S60">
+        <v>86</v>
+      </c>
+      <c r="U60" s="24">
+        <v>0.39</v>
+      </c>
+      <c r="W60" s="28">
+        <v>2754</v>
+      </c>
+      <c r="Y60" s="24">
+        <v>5317.89</v>
+      </c>
+      <c r="AA60" s="24">
+        <v>0.96440999999999999</v>
+      </c>
+      <c r="AC60">
+        <v>4.5</v>
+      </c>
+      <c r="AE60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -7119,6 +7362,11 @@
   <mergeCells count="1">
     <mergeCell ref="AR4:AS4"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F60" r:id="rId1" display="https://ui.adsabs.harvard.edu/abs/2018A&amp;A...619A...1B/abstract" xr:uid="{FA15D441-6A23-1042-8CA6-92DC4EE901BC}"/>
+    <hyperlink ref="H60" r:id="rId2" display="https://ui.adsabs.harvard.edu/abs/2018A&amp;A...619A...1B/abstract" xr:uid="{F11B5C20-2AB0-7B43-B2C8-80B4CE6B3A86}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>